<commit_message>
A few final changes
</commit_message>
<xml_diff>
--- a/figures_tables/table1_formatted_regional_patterns.xlsx
+++ b/figures_tables/table1_formatted_regional_patterns.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahrempel/My Drive/Research_Archives/ecological_drivers_corallivory/figures_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712A2C62-0F4C-C54E-B0C8-8FE3568D304C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7144657-57DE-0F45-9465-D8FB4FB430FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13060" yWindow="500" windowWidth="28180" windowHeight="18700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37100" yWindow="2160" windowWidth="24880" windowHeight="19040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Table 2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Region</t>
   </si>
@@ -130,6 +131,69 @@
       <t xml:space="preserve"> coral)</t>
     </r>
   </si>
+  <si>
+    <t>Scale of inference</t>
+  </si>
+  <si>
+    <t>Scale at which the factor of interest is applied</t>
+  </si>
+  <si>
+    <t>Number of replicates at the appropriate scale</t>
+  </si>
+  <si>
+    <t>Site</t>
+  </si>
+  <si>
+    <t>Regional scale</t>
+  </si>
+  <si>
+    <t>Coral colony</t>
+  </si>
+  <si>
+    <t>4 Greater Caribbean regions (Panamá, Florida, St. Croix, and Bonaire)</t>
+  </si>
+  <si>
+    <t>Sites within regions</t>
+  </si>
+  <si>
+    <t>Panamá: 2 transects per site across 10 sites (n=20 total), Florida: 2-4 transects per site across 4 sites (n=11 total), St. Croix: 5-11 transects per site across 8 sites (n=64 total), Bonaire: 8 transects per site across 4 sites (n=32 total); grand total of 127 transects</t>
+  </si>
+  <si>
+    <t>10 sites in Panamá, 4 sites in Florida, 8 sites in St. Croix, 8 sites in Bonaire; grand total of 30 sites</t>
+  </si>
+  <si>
+    <t>23,075 target coral colonies, of which 323 has recent parrotfish predation scars</t>
+  </si>
+  <si>
+    <t>Transects within sites and regions</t>
+  </si>
+  <si>
+    <r>
+      <t>30 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reef areas</t>
+    </r>
+  </si>
+  <si>
+    <t>Individual colonies within transects, sites, and regions</t>
+  </si>
 </sst>
 </file>
 
@@ -139,7 +203,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -287,6 +351,26 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="46">
     <fill>
@@ -547,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -689,6 +773,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -734,7 +829,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -864,6 +959,24 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1233,11 +1346,594 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4F3B2F7-D6B2-0042-9670-DE3E7BE6CF21}">
+  <dimension ref="A1:K41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+    </row>
+    <row r="2" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+    </row>
+    <row r="3" spans="1:11" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+    </row>
+    <row r="4" spans="1:11" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+    </row>
+    <row r="5" spans="1:11" ht="43" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="44"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="44"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
+      <c r="J13" s="44"/>
+      <c r="K13" s="44"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="44"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="44"/>
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="44"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="44"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="44"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="44"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="44"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="44"/>
+      <c r="G24" s="44"/>
+      <c r="H24" s="44"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="44"/>
+      <c r="K24" s="44"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="44"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="44"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="44"/>
+      <c r="B26" s="44"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="44"/>
+      <c r="K27" s="44"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="44"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="44"/>
+      <c r="G28" s="44"/>
+      <c r="H28" s="44"/>
+      <c r="I28" s="44"/>
+      <c r="J28" s="44"/>
+      <c r="K28" s="44"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
+      <c r="K29" s="44"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="44"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
+      <c r="K30" s="44"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="44"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="44"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="44"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="44"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="44"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="44"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="44"/>
+      <c r="J33" s="44"/>
+      <c r="K33" s="44"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="44"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="44"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="44"/>
+      <c r="I36" s="44"/>
+      <c r="J36" s="44"/>
+      <c r="K36" s="44"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="44"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
+      <c r="G37" s="44"/>
+      <c r="H37" s="44"/>
+      <c r="I37" s="44"/>
+      <c r="J37" s="44"/>
+      <c r="K37" s="44"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="44"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="44"/>
+      <c r="J38" s="44"/>
+      <c r="K38" s="44"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="44"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="44"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="44"/>
+      <c r="I39" s="44"/>
+      <c r="J39" s="44"/>
+      <c r="K39" s="44"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="44"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="44"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="44"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
+      <c r="K40" s="44"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="44"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="44"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView zoomScale="115" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>